<commit_message>
fix: mejorar manejo de caché y validación de datos- Agregar versión al caché de productos (1.0)- Corregir validación de clientes en grupos_clientes.json- Ajustar formato de códigos de cliente en json (sin ceros leading)- Mejorar logs para debugging de caché y productos
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -109,11 +109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,7 +401,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,42 +474,47 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
+      <c r="A2" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(precios): corrige getPrice para retornar precio directo sin acceso a lista de precios- Elimina acceso innecesario a precios[priceList] - Retorna valor directo de product.precio- Los precios ya están filtrados por lista al cargarlos
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="GRUPO_SINPAR" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>evol1970</t>
-  </si>
-  <si>
-    <t>evol115la</t>
   </si>
   <si>
     <t>evo115tu</t>
@@ -400,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,9 +442,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -459,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -480,42 +475,42 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios de nombres de los grupos dentro del archivo catalogo_grupos.xlsx
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GRUPO_SINPAR" sheetId="1" r:id="rId1"/>
-    <sheet name="GRUPO_MAYORISTAS" sheetId="2" r:id="rId2"/>
+    <sheet name="MEJORAR" sheetId="1" r:id="rId1"/>
+    <sheet name="PREMIUM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -397,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -454,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se subio imagen al excel de imagenes, se actualizo token.pickle que permite acceder a la car´peta drive desde app, se actualizaron los json
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="MEJORAR" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>evol0435</t>
+  </si>
+  <si>
+    <t>evol1000</t>
+  </si>
+  <si>
+    <t>PERFA0261</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +419,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -423,26 +429,38 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -452,10 +470,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,47 +487,62 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
+      <c r="A5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agregaron imagenes al drive, tambien se actualizaron los .json
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -52,9 +52,6 @@
     <t>evol3510</t>
   </si>
   <si>
-    <t>evorieg153</t>
-  </si>
-  <si>
     <t>evol0070</t>
   </si>
   <si>
@@ -71,6 +68,69 @@
   </si>
   <si>
     <t>PERFA0261</t>
+  </si>
+  <si>
+    <t>SIM18310</t>
+  </si>
+  <si>
+    <t>KIMERAC1</t>
+  </si>
+  <si>
+    <t>PROBOT41</t>
+  </si>
+  <si>
+    <t>evorieg0153</t>
+  </si>
+  <si>
+    <t>EGWX 01</t>
+  </si>
+  <si>
+    <t>EGWX 02</t>
+  </si>
+  <si>
+    <t>PX120314</t>
+  </si>
+  <si>
+    <t>GAG12103AR</t>
+  </si>
+  <si>
+    <t>TOR01522</t>
+  </si>
+  <si>
+    <t>evol0111</t>
+  </si>
+  <si>
+    <t>evol3970</t>
+  </si>
+  <si>
+    <t>evol0177</t>
+  </si>
+  <si>
+    <t>evol0174</t>
+  </si>
+  <si>
+    <t>evol2205</t>
+  </si>
+  <si>
+    <t>evol1361</t>
+  </si>
+  <si>
+    <t>evol3210</t>
+  </si>
+  <si>
+    <t>evol5530</t>
+  </si>
+  <si>
+    <t>evo115co</t>
+  </si>
+  <si>
+    <t>CON205</t>
+  </si>
+  <si>
+    <t>TF414</t>
+  </si>
+  <si>
+    <t>evo115la</t>
   </si>
 </sst>
 </file>
@@ -112,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -120,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,65 +464,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +686,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +701,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -498,7 +711,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -523,27 +736,27 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoras en el procesamiento de imágenes del catálogo- Modificado drive_scanner.py para incluir columna 'articulo' con el nombre de archivo sin extensión- Corregido process_image_catalog_local() para usar 'articulo' e 'id' como columnas- Modificado process_image_catalog() para reemplazar JSON en lugar de combinar- Evitada duplicación de imágenes entre Excel local y Google Sheets- Agregado mejor manejo de errores y conflictos de Git- Implementado sistema para preservar todas las imágenes (43 en total)- Mejorada la depuración con mensajes más informativos
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>evo115la</t>
+  </si>
+  <si>
+    <t>GAG1685AR</t>
+  </si>
+  <si>
+    <t>GAG12301AR</t>
+  </si>
+  <si>
+    <t>ISAALAMF16</t>
+  </si>
+  <si>
+    <t>EA5310MT</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,6 +195,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A44" sqref="A41:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,6 +688,26 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoras en catálogo de productos:- Corrección de problemas con productos no encontrados- Visualización de 'producto fuera de lista' para artículos no disponibles- Precio .00 para productos sin información- Eliminación de efecto de arrastre entre productos- Mejora en el manejo de errores para productos no encontrados
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -127,22 +127,19 @@
     <t>CON205</t>
   </si>
   <si>
-    <t>TF414</t>
-  </si>
-  <si>
     <t>evo115la</t>
   </si>
   <si>
     <t>GAG1685AR</t>
   </si>
   <si>
-    <t>GAG12301AR</t>
-  </si>
-  <si>
     <t>ISAALAMF16</t>
   </si>
   <si>
     <t>EA5310MT</t>
+  </si>
+  <si>
+    <t>TF.414</t>
   </si>
 </sst>
 </file>
@@ -479,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A44" sqref="A41:A44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +589,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -687,27 +684,22 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementado diseño masonry con CSS columns, mejorada la tipografía y reducido el espaciado vertical entre elementos
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>TF.414</t>
+  </si>
+  <si>
+    <t>EVOL3975</t>
   </si>
 </sst>
 </file>
@@ -476,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +703,11 @@
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion: imagenes al catalogo
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -143,6 +143,27 @@
   </si>
   <si>
     <t>EVOL3975</t>
+  </si>
+  <si>
+    <t>SAHANAF1H</t>
+  </si>
+  <si>
+    <t>SAHANAF2H</t>
+  </si>
+  <si>
+    <t>EVOL0043</t>
+  </si>
+  <si>
+    <t>EVOL3420</t>
+  </si>
+  <si>
+    <t>EVOL5530</t>
+  </si>
+  <si>
+    <t>EVOL4755</t>
+  </si>
+  <si>
+    <t>EVOL4753</t>
   </si>
 </sst>
 </file>
@@ -479,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +729,41 @@
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se sumaron mas imagenes al catalogo
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -118,9 +118,6 @@
     <t>evol3210</t>
   </si>
   <si>
-    <t>evol5530</t>
-  </si>
-  <si>
     <t>evo115co</t>
   </si>
   <si>
@@ -164,6 +161,33 @@
   </si>
   <si>
     <t>EVOL4753</t>
+  </si>
+  <si>
+    <t>EVOL0144</t>
+  </si>
+  <si>
+    <t>EVOL5100</t>
+  </si>
+  <si>
+    <t>EVOL0340</t>
+  </si>
+  <si>
+    <t>EVOL0108</t>
+  </si>
+  <si>
+    <t>EVOL1200</t>
+  </si>
+  <si>
+    <t>EVOL1631</t>
+  </si>
+  <si>
+    <t>EVOL2135</t>
+  </si>
+  <si>
+    <t>EVOL0135</t>
+  </si>
+  <si>
+    <t>EVOL1208</t>
   </si>
 </sst>
 </file>
@@ -500,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +637,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -703,12 +727,12 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>39</v>
+      <c r="A40" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -722,8 +746,8 @@
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>38</v>
+      <c r="A43" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -764,6 +788,46 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementación de layout Pinterest con optimizaciones para evitar superposición inicial de imágenes
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -124,9 +124,6 @@
     <t>CON205</t>
   </si>
   <si>
-    <t>evo115la</t>
-  </si>
-  <si>
     <t>GAG1685AR</t>
   </si>
   <si>
@@ -188,6 +185,60 @@
   </si>
   <si>
     <t>EVOL1208</t>
+  </si>
+  <si>
+    <t>EVOL0224</t>
+  </si>
+  <si>
+    <t>EVO115TF</t>
+  </si>
+  <si>
+    <t>EVO180LA</t>
+  </si>
+  <si>
+    <t>EVO180CO</t>
+  </si>
+  <si>
+    <t>EVO115LA</t>
+  </si>
+  <si>
+    <t>EVO230CO</t>
+  </si>
+  <si>
+    <t>EVO180TU</t>
+  </si>
+  <si>
+    <t>EVO230TU</t>
+  </si>
+  <si>
+    <t>EVOL2200</t>
+  </si>
+  <si>
+    <t>EVOL2205</t>
+  </si>
+  <si>
+    <t>EVOL2210</t>
+  </si>
+  <si>
+    <t>EVOL2213</t>
+  </si>
+  <si>
+    <t>EVOL2215</t>
+  </si>
+  <si>
+    <t>EVOL1160</t>
+  </si>
+  <si>
+    <t>EVOL1165</t>
+  </si>
+  <si>
+    <t>EVOL1150</t>
+  </si>
+  <si>
+    <t>EVOL1152</t>
+  </si>
+  <si>
+    <t>EVOL1154</t>
   </si>
 </sst>
 </file>
@@ -229,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,6 +294,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:A76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,97 +691,97 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>38</v>
+      <c r="A39" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -741,8 +795,8 @@
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>37</v>
+      <c r="A42" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -828,6 +882,91 @@
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se han subidos nuevas imagenes para el catalogo
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="182">
   <si>
     <t>Codigo_Producto</t>
   </si>
@@ -31,9 +31,6 @@
     <t>evol0330</t>
   </si>
   <si>
-    <t>evol3089</t>
-  </si>
-  <si>
     <t>evol0025</t>
   </si>
   <si>
@@ -239,6 +236,336 @@
   </si>
   <si>
     <t>EVOL1154</t>
+  </si>
+  <si>
+    <t>EVOL4050</t>
+  </si>
+  <si>
+    <t>EVOL4000</t>
+  </si>
+  <si>
+    <t>EVOL0138</t>
+  </si>
+  <si>
+    <t>EVOL0139</t>
+  </si>
+  <si>
+    <t>EVOL0071</t>
+  </si>
+  <si>
+    <t>EVOL0070</t>
+  </si>
+  <si>
+    <t>EVOL0223</t>
+  </si>
+  <si>
+    <t>EVOL0320</t>
+  </si>
+  <si>
+    <t>EVOL0033</t>
+  </si>
+  <si>
+    <t>EVOL0089</t>
+  </si>
+  <si>
+    <t>EVOL3415</t>
+  </si>
+  <si>
+    <t>EVOL1351</t>
+  </si>
+  <si>
+    <t>EVOL1331</t>
+  </si>
+  <si>
+    <t>EVOL0229</t>
+  </si>
+  <si>
+    <t>EVOL0145</t>
+  </si>
+  <si>
+    <t>EVOL0146</t>
+  </si>
+  <si>
+    <t>EVOL0147</t>
+  </si>
+  <si>
+    <t>EVOL0148</t>
+  </si>
+  <si>
+    <t>EVOL0044</t>
+  </si>
+  <si>
+    <t>EVOL0045</t>
+  </si>
+  <si>
+    <t>EVOMYR1928</t>
+  </si>
+  <si>
+    <t>EVOMYR1929</t>
+  </si>
+  <si>
+    <t>EVOMYR1931</t>
+  </si>
+  <si>
+    <t>EVOMYR1927</t>
+  </si>
+  <si>
+    <t>EVOL0249</t>
+  </si>
+  <si>
+    <t>EVOL0248</t>
+  </si>
+  <si>
+    <t>EVOL0211</t>
+  </si>
+  <si>
+    <t>EVOL1470</t>
+  </si>
+  <si>
+    <t>EVOMYR5807</t>
+  </si>
+  <si>
+    <t>EVOMYR5808</t>
+  </si>
+  <si>
+    <t>EVOMYR5810</t>
+  </si>
+  <si>
+    <t>EVOL1429</t>
+  </si>
+  <si>
+    <t>EVOL1430</t>
+  </si>
+  <si>
+    <t>EVOL1960</t>
+  </si>
+  <si>
+    <t>EVOL0001</t>
+  </si>
+  <si>
+    <t>EVOL0086</t>
+  </si>
+  <si>
+    <t>EVOL0021</t>
+  </si>
+  <si>
+    <t>EVOL0022</t>
+  </si>
+  <si>
+    <t>EVOL0023</t>
+  </si>
+  <si>
+    <t>EVOL0024</t>
+  </si>
+  <si>
+    <t>EVOL0208</t>
+  </si>
+  <si>
+    <t>EVOL0028</t>
+  </si>
+  <si>
+    <t>EVOL0218</t>
+  </si>
+  <si>
+    <t>EVOL0214</t>
+  </si>
+  <si>
+    <t>EVOL0215</t>
+  </si>
+  <si>
+    <t>EVOL0216</t>
+  </si>
+  <si>
+    <t>EVOL0217</t>
+  </si>
+  <si>
+    <t>EVOL4900</t>
+  </si>
+  <si>
+    <t>EVOL4910</t>
+  </si>
+  <si>
+    <t>EVOL4920</t>
+  </si>
+  <si>
+    <t>EVOL4930</t>
+  </si>
+  <si>
+    <t>EVOL0234</t>
+  </si>
+  <si>
+    <t>EVOL0030</t>
+  </si>
+  <si>
+    <t>EVOL1776</t>
+  </si>
+  <si>
+    <t>EVOL0002</t>
+  </si>
+  <si>
+    <t>EVOL1772</t>
+  </si>
+  <si>
+    <t>EVOL0035</t>
+  </si>
+  <si>
+    <t>EVOL1096</t>
+  </si>
+  <si>
+    <t>EVOL1097</t>
+  </si>
+  <si>
+    <t>EVOL1770</t>
+  </si>
+  <si>
+    <t>EVOL1768</t>
+  </si>
+  <si>
+    <t>EVOL0006</t>
+  </si>
+  <si>
+    <t>EVOL0007</t>
+  </si>
+  <si>
+    <t>EVOL0096</t>
+  </si>
+  <si>
+    <t>EVOL0097</t>
+  </si>
+  <si>
+    <t>EVOL1774</t>
+  </si>
+  <si>
+    <t>EVOL0003</t>
+  </si>
+  <si>
+    <t>EVOL0004</t>
+  </si>
+  <si>
+    <t>EVOL0130</t>
+  </si>
+  <si>
+    <t>EVOL3700</t>
+  </si>
+  <si>
+    <t>EVOL3710</t>
+  </si>
+  <si>
+    <t>EVOL3720</t>
+  </si>
+  <si>
+    <t>EVOL3730</t>
+  </si>
+  <si>
+    <t>EVOL3740</t>
+  </si>
+  <si>
+    <t>EVOL3800</t>
+  </si>
+  <si>
+    <t>EVOL3810</t>
+  </si>
+  <si>
+    <t>EVOL3820</t>
+  </si>
+  <si>
+    <t>EVOL0192</t>
+  </si>
+  <si>
+    <t>EVOL3620</t>
+  </si>
+  <si>
+    <t>EVOL3630</t>
+  </si>
+  <si>
+    <t>EVOL3650</t>
+  </si>
+  <si>
+    <t>EVOL0400</t>
+  </si>
+  <si>
+    <t>EVOL0410</t>
+  </si>
+  <si>
+    <t>EVOL0440</t>
+  </si>
+  <si>
+    <t>EVOL0420</t>
+  </si>
+  <si>
+    <t>EVOL0430</t>
+  </si>
+  <si>
+    <t>EVOL0460</t>
+  </si>
+  <si>
+    <t>EVOL0470</t>
+  </si>
+  <si>
+    <t>EVOL0094</t>
+  </si>
+  <si>
+    <t>EVOL0095</t>
+  </si>
+  <si>
+    <t>EVOL3089</t>
+  </si>
+  <si>
+    <t>EVOL3086</t>
+  </si>
+  <si>
+    <t>EVOL3087</t>
+  </si>
+  <si>
+    <t>EVOL3088</t>
+  </si>
+  <si>
+    <t>EVOL3961</t>
+  </si>
+  <si>
+    <t>EVOL3955</t>
+  </si>
+  <si>
+    <t>EVOL3959</t>
+  </si>
+  <si>
+    <t>EVOL3953</t>
+  </si>
+  <si>
+    <t>EVOL3957</t>
+  </si>
+  <si>
+    <t>EVOL6205</t>
+  </si>
+  <si>
+    <t>EVOL6210</t>
+  </si>
+  <si>
+    <t>EVOL6221</t>
+  </si>
+  <si>
+    <t>EVOL6222</t>
+  </si>
+  <si>
+    <t>EVOL6715</t>
+  </si>
+  <si>
+    <t>EVOL6760</t>
+  </si>
+  <si>
+    <t>EVOL6765</t>
+  </si>
+  <si>
+    <t>EVOL0008</t>
+  </si>
+  <si>
+    <t>EVOL0009</t>
+  </si>
+  <si>
+    <t>EVOL0010</t>
+  </si>
+  <si>
+    <t>EVOL0011</t>
   </si>
 </sst>
 </file>
@@ -578,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:A76"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A181" sqref="A181:A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,37 +923,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -636,7 +963,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -646,17 +973,17 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -701,7 +1028,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -721,17 +1048,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -771,12 +1098,12 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -790,8 +1117,8 @@
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>36</v>
+      <c r="A41" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -940,7 +1267,7 @@
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="6" t="s">
         <v>67</v>
       </c>
     </row>
@@ -967,6 +1294,546 @@
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -995,7 +1862,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1005,7 +1872,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -1015,42 +1882,42 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corregi errores en el algunos codigos new clor
</commit_message>
<xml_diff>
--- a/excel/CATALOGO_GRUPOS.xlsx
+++ b/excel/CATALOGO_GRUPOS.xlsx
@@ -17,7 +17,7 @@
     <sheet name="RECURRENTE_400K-500K" sheetId="8" r:id="rId8"/>
     <sheet name="RECURRENTE_&gt;_500K" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -719,19 +719,19 @@
     <t>ROT98001</t>
   </si>
   <si>
-    <t>NEWCGTA1K</t>
-  </si>
-  <si>
-    <t>NEWCPTA1K</t>
-  </si>
-  <si>
     <t>NEW023400020002</t>
   </si>
   <si>
-    <t>NEW010911K00000</t>
-  </si>
-  <si>
-    <t>NEW010921K00000</t>
+    <t>NEWCALGUI</t>
+  </si>
+  <si>
+    <t>NEWCCLARI</t>
+  </si>
+  <si>
+    <t>NEWCGTAG1K</t>
+  </si>
+  <si>
+    <t>NEWCPTAG200G</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,27 +1116,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -2279,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A238"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A238"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,27 +2325,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -3533,27 +3533,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -4741,27 +4741,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -5949,27 +5949,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -7157,27 +7157,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -8365,27 +8365,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -9573,27 +9573,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -10781,27 +10781,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>